<commit_message>
Fin du développement de la classe Salle
</commit_message>
<xml_diff>
--- a/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
+++ b/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
   <si>
     <t>A faire</t>
   </si>
@@ -217,10 +217,10 @@
     <t>Tous</t>
   </si>
   <si>
-    <t>Matte-hieux</t>
-  </si>
-  <si>
     <t>Thomas</t>
+  </si>
+  <si>
+    <t>Mathieu</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,16 +813,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="F17" s="7">
+        <v>42640</v>
+      </c>
+      <c r="G17" s="7">
+        <v>42640</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -879,7 +885,7 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>

</xml_diff>

<commit_message>
Modif fichier des taches existeReservation
</commit_message>
<xml_diff>
--- a/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
+++ b/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11055" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -658,7 +658,7 @@
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -982,17 +982,13 @@
       <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="7">
-        <v>42647</v>
-      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
@@ -1001,10 +997,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E29" s="5" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Création fonction existeReservation Modification Excel
</commit_message>
<xml_diff>
--- a/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
+++ b/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23115" windowHeight="10665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -658,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,30 +980,28 @@
       <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="7">
-        <v>42647</v>
-      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1111,9 +1109,7 @@
       <c r="D35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="7">
         <v>42640</v>
@@ -1124,11 +1120,11 @@
       <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>

</xml_diff>

<commit_message>
Vue et Ctrl SupprimerUtilisateur
</commit_message>
<xml_diff>
--- a/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
+++ b/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="10665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -658,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,29 +1511,41 @@
       <c r="A62" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+      <c r="G62" s="7">
+        <v>42682</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B63" s="5"/>
       <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="G63" s="7">
+        <v>42682</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>

</xml_diff>

<commit_message>
Controleur changerMdp Vue changerMdp
</commit_message>
<xml_diff>
--- a/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
+++ b/m.m2l.incomplet/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="70">
   <si>
     <t>A faire</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Thomas</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -658,8 +661,8 @@
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,12 +1342,14 @@
       <c r="A50" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
@@ -1353,12 +1358,14 @@
       <c r="A51" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>

</xml_diff>